<commit_message>
worked on excel reading
</commit_message>
<xml_diff>
--- a/TestData1.xlsx
+++ b/TestData1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andres\Documents\HTML\HTML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres\Documents\HTML\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC397DB7-8FFF-49E7-90AD-720562EACAC0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8505"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -335,164 +336,164 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:L8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B1">
         <v>65</v>
       </c>
-      <c r="C5">
+      <c r="C1">
         <v>35</v>
       </c>
-      <c r="D5">
+      <c r="D1">
         <v>68</v>
       </c>
-      <c r="E5">
+      <c r="E1">
         <v>33</v>
       </c>
-      <c r="F5">
+      <c r="F1">
         <v>79</v>
       </c>
-      <c r="G5">
+      <c r="G1">
         <v>35</v>
       </c>
-      <c r="H5">
+      <c r="H1">
         <v>69</v>
       </c>
-      <c r="I5">
+      <c r="I1">
         <v>75</v>
       </c>
-      <c r="J5">
+      <c r="J1">
         <v>65</v>
       </c>
-      <c r="K5">
+      <c r="K1">
         <v>98</v>
       </c>
-      <c r="L5">
+      <c r="L1">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>50</v>
       </c>
-      <c r="B6">
+      <c r="B2">
         <v>65</v>
       </c>
-      <c r="C6">
+      <c r="C2">
         <v>25</v>
       </c>
-      <c r="D6">
+      <c r="D2">
         <v>59</v>
       </c>
-      <c r="E6">
+      <c r="E2">
         <v>21</v>
       </c>
-      <c r="F6">
+      <c r="F2">
         <v>94</v>
       </c>
-      <c r="G6">
+      <c r="G2">
         <v>31</v>
       </c>
-      <c r="H6">
+      <c r="H2">
         <v>64</v>
       </c>
-      <c r="I6">
+      <c r="I2">
         <v>41</v>
       </c>
-      <c r="J6">
+      <c r="J2">
         <v>65</v>
       </c>
-      <c r="K6">
+      <c r="K2">
         <v>65</v>
       </c>
-      <c r="L6">
+      <c r="L2">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>24</v>
       </c>
-      <c r="B7">
+      <c r="B3">
         <v>15</v>
       </c>
-      <c r="C7">
+      <c r="C3">
         <v>52</v>
       </c>
-      <c r="D7">
+      <c r="D3">
         <v>31</v>
       </c>
-      <c r="E7">
+      <c r="E3">
         <v>15</v>
       </c>
-      <c r="F7">
+      <c r="F3">
         <v>27</v>
       </c>
-      <c r="G7">
+      <c r="G3">
         <v>63</v>
       </c>
-      <c r="H7">
+      <c r="H3">
         <v>85</v>
       </c>
-      <c r="I7">
+      <c r="I3">
         <v>23</v>
       </c>
-      <c r="J7">
+      <c r="J3">
         <v>78</v>
       </c>
-      <c r="K7">
+      <c r="K3">
         <v>12</v>
       </c>
-      <c r="L7">
+      <c r="L3">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B4">
         <v>132</v>
       </c>
-      <c r="C8">
+      <c r="C4">
         <v>75</v>
       </c>
-      <c r="D8">
+      <c r="D4">
         <v>91</v>
       </c>
-      <c r="E8">
+      <c r="E4">
         <v>17</v>
       </c>
-      <c r="F8">
+      <c r="F4">
         <v>18</v>
       </c>
-      <c r="G8">
+      <c r="G4">
         <v>87</v>
       </c>
-      <c r="H8">
+      <c r="H4">
         <v>25</v>
       </c>
-      <c r="I8">
+      <c r="I4">
         <v>38</v>
       </c>
-      <c r="J8">
+      <c r="J4">
         <v>14</v>
       </c>
-      <c r="K8">
+      <c r="K4">
         <v>56</v>
       </c>
-      <c r="L8">
+      <c r="L4">
         <v>32</v>
       </c>
     </row>

</xml_diff>